<commit_message>
Fix data entry errors for Peter Douthwright (2020-03-17)
</commit_message>
<xml_diff>
--- a/data/2020-03-17/Senior Cubers Worldwide - Weekly Competition - 2020-03-17.xlsx
+++ b/data/2020-03-17/Senior Cubers Worldwide - Weekly Competition - 2020-03-17.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-03-17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD305438-268A-4916-A455-8959C9EE7C19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A58659-89BF-41D1-A4C7-1AA2496BDE85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3x3x3" sheetId="1" r:id="rId1"/>
@@ -632,6 +632,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="25">
     <font>
       <sz val="10"/>
@@ -800,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -969,6 +972,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
@@ -1191,8 +1197,8 @@
   </sheetPr>
   <dimension ref="A1:N1074"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2213,27 +2219,27 @@
       <c r="C28" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="19">
-        <v>44.692999999999998</v>
-      </c>
-      <c r="E28" s="19">
+      <c r="D28" s="74">
+        <v>44.826999999999998</v>
+      </c>
+      <c r="E28" s="74">
         <v>38.828000000000003</v>
       </c>
       <c r="F28" s="17"/>
-      <c r="G28" s="19">
-        <v>45.29</v>
-      </c>
-      <c r="H28" s="19">
-        <v>45.48</v>
-      </c>
-      <c r="I28" s="19">
-        <v>43.32</v>
-      </c>
-      <c r="J28" s="19">
-        <v>46.88</v>
-      </c>
-      <c r="K28" s="19">
-        <v>38.83</v>
+      <c r="G28" s="74">
+        <v>45.284999999999997</v>
+      </c>
+      <c r="H28" s="74">
+        <v>45.877000000000002</v>
+      </c>
+      <c r="I28" s="74">
+        <v>43.317999999999998</v>
+      </c>
+      <c r="J28" s="74">
+        <v>46.881</v>
+      </c>
+      <c r="K28" s="74">
+        <v>38.828000000000003</v>
       </c>
       <c r="L28" s="22" t="s">
         <v>179</v>
@@ -14854,8 +14860,8 @@
   </sheetPr>
   <dimension ref="A1:M1051"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -32733,12 +32739,12 @@
       <c r="A1" s="63" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
       <c r="F1" s="64"/>
     </row>
     <row r="2" spans="1:7" ht="12.75">

</xml_diff>